<commit_message>
📊 回線モニタシステムデータ更新 [2025/8/14] by Markov - 2025/08/14 13:05:08
</commit_message>
<xml_diff>
--- a/data/回線モニタシステム[R320e-E4]HW監視作業履歴.xlsx
+++ b/data/回線モニタシステム[R320e-E4]HW監視作業履歴.xlsx
@@ -1035,7 +1035,7 @@
       </c>
       <c r="Z2" s="3" t="inlineStr">
         <is>
-          <t>2025-08-14 04:02:35</t>
+          <t>2025-08-14 04:05:07</t>
         </is>
       </c>
     </row>
@@ -1128,7 +1128,11 @@
       <c r="W5" s="5" t="n"/>
       <c r="X5" s="5" t="n"/>
       <c r="Y5" s="6" t="n"/>
-      <c r="Z5" s="121" t="n"/>
+      <c r="Z5" s="121" t="inlineStr">
+        <is>
+          <t>hoge</t>
+        </is>
+      </c>
     </row>
     <row r="6" customFormat="1" s="2">
       <c r="B6" s="122" t="n"/>
@@ -1137,7 +1141,7 @@
       <c r="E6" s="7" t="n"/>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>CPUモジュール、PCIモジュール：</t>
+          <t>Duplex</t>
         </is>
       </c>
       <c r="P6" s="66" t="inlineStr">
@@ -1157,7 +1161,7 @@
       <c r="E7" s="7" t="n"/>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>SCSIエンクロージャ：</t>
+          <t>Online</t>
         </is>
       </c>
       <c r="P7" s="67" t="inlineStr">
@@ -1229,7 +1233,7 @@
         </is>
       </c>
       <c r="G12" s="125" t="n">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="H12" s="123" t="n"/>
       <c r="I12" s="123" t="n"/>
@@ -1267,7 +1271,7 @@
         </is>
       </c>
       <c r="G13" s="125" t="n">
-        <v>278</v>
+        <v>23</v>
       </c>
       <c r="H13" s="123" t="n"/>
       <c r="I13" s="123" t="n"/>
@@ -1299,6 +1303,9 @@
       <c r="C14" s="122" t="n"/>
       <c r="D14" s="122" t="n"/>
       <c r="E14" s="7" t="n"/>
+      <c r="G14" t="n">
+        <v>44</v>
+      </c>
       <c r="Y14" s="8" t="n"/>
       <c r="Z14" s="122" t="n"/>
     </row>
@@ -1310,6 +1317,9 @@
         <is>
           <t>タスクマネージャ：</t>
         </is>
+      </c>
+      <c r="G15" t="n">
+        <v>32</v>
       </c>
       <c r="Y15" s="8" t="n"/>
       <c r="Z15" s="122" t="n"/>
@@ -1324,10 +1334,8 @@
           <t>メモリ使用量：</t>
         </is>
       </c>
-      <c r="J16" s="2" t="inlineStr">
-        <is>
-          <t>w3wp.exeの使用量</t>
-        </is>
+      <c r="J16" s="2" t="n">
+        <v>32</v>
       </c>
       <c r="U16" s="125" t="n">
         <v>539.6</v>
@@ -1347,10 +1355,8 @@
       <c r="C17" s="122" t="n"/>
       <c r="D17" s="122" t="n"/>
       <c r="E17" s="7" t="n"/>
-      <c r="J17" s="2" t="inlineStr">
-        <is>
-          <t>SQLServe：</t>
-        </is>
+      <c r="J17" s="2" t="n">
+        <v>21</v>
       </c>
       <c r="P17" s="126" t="n"/>
       <c r="Q17" s="126" t="n"/>
@@ -1363,6 +1369,9 @@
       <c r="C18" s="122" t="n"/>
       <c r="D18" s="122" t="n"/>
       <c r="E18" s="7" t="n"/>
+      <c r="J18" t="n">
+        <v>12</v>
+      </c>
       <c r="K18" s="2" t="inlineStr">
         <is>
           <t>MSSQL$KAISENMONITOR：</t>
@@ -1412,10 +1421,8 @@
       <c r="C20" s="122" t="n"/>
       <c r="D20" s="122" t="n"/>
       <c r="E20" s="7" t="n"/>
-      <c r="J20" s="2" t="inlineStr">
-        <is>
-          <t>全体メモリ使用量：</t>
-        </is>
+      <c r="J20" s="2" t="n">
+        <v>33</v>
       </c>
       <c r="P20" s="127" t="n">
         <v>6.9</v>
@@ -1435,10 +1442,8 @@
       <c r="C21" s="122" t="n"/>
       <c r="D21" s="122" t="n"/>
       <c r="E21" s="7" t="n"/>
-      <c r="F21" s="2" t="inlineStr">
-        <is>
-          <t>CPU使用率：</t>
-        </is>
+      <c r="F21" s="2" t="n">
+        <v>2</v>
       </c>
       <c r="J21" s="71" t="n">
         <v>0</v>
@@ -1450,8 +1455,10 @@
           <t xml:space="preserve">[%] </t>
         </is>
       </c>
-      <c r="P21" s="72" t="n">
-        <v>0.6076388888888888</v>
+      <c r="P21" s="72" t="inlineStr">
+        <is>
+          <t>13:05</t>
+        </is>
       </c>
       <c r="Q21" s="123" t="n"/>
       <c r="R21" s="123" t="n"/>
@@ -1468,7 +1475,11 @@
       <c r="C22" s="122" t="n"/>
       <c r="D22" s="122" t="n"/>
       <c r="E22" s="7" t="n"/>
-      <c r="J22" s="78" t="n"/>
+      <c r="J22" s="78" t="inlineStr">
+        <is>
+          <t>99</t>
+        </is>
+      </c>
       <c r="K22" s="78" t="n"/>
       <c r="L22" s="78" t="n"/>
       <c r="P22" s="78" t="n"/>

</xml_diff>

<commit_message>
📊 回線モニタシステムデータ更新 [2025/8/14] by Markov - 2025/08/14 13:11:45
</commit_message>
<xml_diff>
--- a/data/回線モニタシステム[R320e-E4]HW監視作業履歴.xlsx
+++ b/data/回線モニタシステム[R320e-E4]HW監視作業履歴.xlsx
@@ -1035,7 +1035,7 @@
       </c>
       <c r="Z2" s="3" t="inlineStr">
         <is>
-          <t>2025-08-14 04:05:07</t>
+          <t>2025-08-14 04:11:45</t>
         </is>
       </c>
     </row>
@@ -1141,7 +1141,7 @@
       <c r="E6" s="7" t="n"/>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>Duplex</t>
+          <t>Simplex</t>
         </is>
       </c>
       <c r="P6" s="66" t="inlineStr">
@@ -1161,7 +1161,7 @@
       <c r="E7" s="7" t="n"/>
       <c r="F7" s="2" t="inlineStr">
         <is>
-          <t>Online</t>
+          <t>Error</t>
         </is>
       </c>
       <c r="P7" s="67" t="inlineStr">
@@ -1193,7 +1193,7 @@
       </c>
       <c r="J9" s="66" t="inlineStr">
         <is>
-          <t>問題なし</t>
+          <t>問題なしs</t>
         </is>
       </c>
       <c r="K9" s="123" t="n"/>
@@ -1233,7 +1233,7 @@
         </is>
       </c>
       <c r="G12" s="125" t="n">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="H12" s="123" t="n"/>
       <c r="I12" s="123" t="n"/>
@@ -1271,7 +1271,7 @@
         </is>
       </c>
       <c r="G13" s="125" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H13" s="123" t="n"/>
       <c r="I13" s="123" t="n"/>
@@ -1304,7 +1304,7 @@
       <c r="D14" s="122" t="n"/>
       <c r="E14" s="7" t="n"/>
       <c r="G14" t="n">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Y14" s="8" t="n"/>
       <c r="Z14" s="122" t="n"/>
@@ -1319,7 +1319,7 @@
         </is>
       </c>
       <c r="G15" t="n">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="Y15" s="8" t="n"/>
       <c r="Z15" s="122" t="n"/>
@@ -1335,7 +1335,7 @@
         </is>
       </c>
       <c r="J16" s="2" t="n">
-        <v>32</v>
+        <v>555</v>
       </c>
       <c r="U16" s="125" t="n">
         <v>539.6</v>
@@ -1370,7 +1370,7 @@
       <c r="D18" s="122" t="n"/>
       <c r="E18" s="7" t="n"/>
       <c r="J18" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="K18" s="2" t="inlineStr">
         <is>
@@ -1422,7 +1422,7 @@
       <c r="D20" s="122" t="n"/>
       <c r="E20" s="7" t="n"/>
       <c r="J20" s="2" t="n">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="P20" s="127" t="n">
         <v>6.9</v>
@@ -1443,7 +1443,7 @@
       <c r="D21" s="122" t="n"/>
       <c r="E21" s="7" t="n"/>
       <c r="F21" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J21" s="71" t="n">
         <v>0</v>
@@ -1457,7 +1457,7 @@
       </c>
       <c r="P21" s="72" t="inlineStr">
         <is>
-          <t>13:05</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="Q21" s="123" t="n"/>
@@ -1477,7 +1477,7 @@
       <c r="E22" s="7" t="n"/>
       <c r="J22" s="78" t="inlineStr">
         <is>
-          <t>99</t>
+          <t>3333</t>
         </is>
       </c>
       <c r="K22" s="78" t="n"/>
@@ -1511,10 +1511,8 @@
       <c r="C24" s="122" t="n"/>
       <c r="D24" s="122" t="n"/>
       <c r="E24" s="7" t="n"/>
-      <c r="F24" s="2" t="inlineStr">
-        <is>
-          <t>上段サーバランプ点灯数：</t>
-        </is>
+      <c r="F24" s="2" t="n">
+        <v>2</v>
       </c>
       <c r="J24" s="78" t="n"/>
       <c r="K24" s="78" t="n"/>
@@ -1539,10 +1537,8 @@
       <c r="C25" s="122" t="n"/>
       <c r="D25" s="122" t="n"/>
       <c r="E25" s="7" t="n"/>
-      <c r="F25" s="2" t="inlineStr">
-        <is>
-          <t>下段サーバランプ点灯数：</t>
-        </is>
+      <c r="F25" s="2" t="n">
+        <v>4</v>
       </c>
       <c r="J25" s="78" t="n"/>
       <c r="K25" s="78" t="n"/>

</xml_diff>